<commit_message>
New updates for Admin and institute
</commit_message>
<xml_diff>
--- a/EvolvedTax_Institute/wwwroot/Templates/New_Partner_Template.xlsx
+++ b/EvolvedTax_Institute/wwwroot/Templates/New_Partner_Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\EvoTaxPortal\EvolvedTax_Institute\wwwroot\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D3E8E8-87E2-414C-8702-F7C0C0DB8825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A0B1CF4-0A95-45D6-B94F-1529E4B57355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="314">
   <si>
     <t>City</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>Province (If Applicable)</t>
-  </si>
-  <si>
-    <t>Entity Name</t>
   </si>
   <si>
     <t>Partner Name 1</t>
@@ -1329,20 +1326,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="34.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="34.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="10" width="29.28515625" customWidth="1"/>
-    <col min="11" max="11" width="32.7109375" customWidth="1"/>
-    <col min="12" max="12" width="29.28515625" style="5" customWidth="1"/>
+    <col min="1" max="9" width="29.26953125" customWidth="1"/>
+    <col min="10" max="10" width="32.7265625" customWidth="1"/>
+    <col min="11" max="11" width="29.26953125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1356,37 +1353,34 @@
         <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="I1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="L2" s="6"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K2" s="6"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Valid Email Address" error="Please enter the valid email address" sqref="L1:L1048576" xr:uid="{40F70394-9C27-40A1-AA84-8CC7F95EE935}">
-      <formula1>ISNUMBER(MATCH("*@*.?*",L:L,0))</formula1>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Valid Email Address" error="Please enter the valid email address" sqref="K1:K1048576" xr:uid="{40F70394-9C27-40A1-AA84-8CC7F95EE935}">
+      <formula1>ISNUMBER(MATCH("*@*.?*",K:K,0))</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1398,13 +1392,13 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$1:$A$253</xm:f>
           </x14:formula1>
-          <xm:sqref>J1:J1048576</xm:sqref>
+          <xm:sqref>I1:I1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{489FE3B5-5F87-4812-9404-1225046F4682}">
           <x14:formula1>
             <xm:f>Sheet2!$B$1:$B$52</xm:f>
           </x14:formula1>
-          <xm:sqref>G1:G1048576</xm:sqref>
+          <xm:sqref>F1:F1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1420,1431 +1414,1431 @@
       <selection activeCell="A234" sqref="A234"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="42.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C2" s="3">
         <f ca="1">TODAY()</f>
-        <v>45231</v>
+        <v>45236</v>
       </c>
       <c r="D2" s="3">
         <v>29221</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B3" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B4" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B5" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B6" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B7" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B8" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B9" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B10" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B11" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B12" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B13" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B14" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B15" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B16" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B17" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B18" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B19" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B20" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B21" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B22" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B23" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B24" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B25" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B26" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B27" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B28" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B29" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B30" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B31" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B32" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B33" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B34" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B35" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B36" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B37" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B38" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B39" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B40" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B41" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B42" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B43" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B44" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B45" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B46" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B47" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B48" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B49" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B50" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B51" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B52" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>